<commit_message>
Missing images & license file
</commit_message>
<xml_diff>
--- a/CT_Sim_Workbook_V1.xlsx
+++ b/CT_Sim_Workbook_V1.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnstowe/Google Drive/Modules/Sem I UGFT RDGY30590 Computed Tomography/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnstowe/CTSim/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D9CE8E-F37C-064F-8C1B-1516283DB3E1}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25020" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25020" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dual Energy" sheetId="3" r:id="rId1"/>
     <sheet name="Doses" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Noise" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -178,7 +179,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -207,6 +208,7 @@
       <sz val="12"/>
       <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -655,9 +657,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -725,6 +724,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -740,12 +742,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -789,7 +794,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -858,22 +862,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90.0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110.0</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120.0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>130.0</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -885,18 +889,23 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>39.0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EEB8-CE41-9B81-21D1E6DC8520}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -943,7 +952,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1064,7 +1072,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1094,6 +1101,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1174,7 +1182,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1213,7 +1221,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1282,22 +1289,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90.0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110.0</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120.0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>130.0</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1309,18 +1316,23 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-32.0</c:v>
+                  <c:v>-70</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-11.0</c:v>
+                  <c:v>-30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.0</c:v>
+                  <c:v>-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4F04-8A44-9060-3EE48C95595A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1367,7 +1379,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1488,7 +1499,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1518,6 +1528,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1598,7 +1609,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1642,7 +1653,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1711,22 +1721,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90.0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110.0</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120.0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>130.0</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1738,18 +1748,23 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>77.0</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74.0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>73.0</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-01EF-6448-ABFC-94B6F73EEAAF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1796,7 +1811,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1917,7 +1931,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1947,6 +1960,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1995,10 +2009,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.248850462962963"/>
-          <c:y val="0.909831712962963"/>
-          <c:w val="0.536151851851852"/>
-          <c:h val="0.0554893518518518"/>
+          <c:x val="0.24885046296296301"/>
+          <c:y val="0.90983171296296295"/>
+          <c:w val="0.53615185185185199"/>
+          <c:h val="5.5489351851851797E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2068,7 +2082,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2112,7 +2126,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2181,22 +2194,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90.0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110.0</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120.0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>130.0</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2208,18 +2221,23 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1192.0</c:v>
+                  <c:v>1192</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>909.0</c:v>
+                  <c:v>909</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>787.0</c:v>
+                  <c:v>787</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-94A5-ED4E-9ECB-B93D3314BD8F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2266,7 +2284,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2387,7 +2404,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2417,6 +2433,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2465,10 +2482,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.248850462962963"/>
-          <c:y val="0.909831712962963"/>
-          <c:w val="0.536151851851852"/>
-          <c:h val="0.0554893518518518"/>
+          <c:x val="0.24885046296296301"/>
+          <c:y val="0.90983171296296295"/>
+          <c:w val="0.53615185185185199"/>
+          <c:h val="5.5489351851851797E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2538,7 +2555,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2577,7 +2594,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2646,7 +2662,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3.905</c:v>
+                  <c:v>3.9049999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7.81</c:v>
@@ -2658,7 +2674,7 @@
                   <c:v>15.62</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>23.43</c:v>
@@ -2670,15 +2686,20 @@
                   <c:v>31.24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.145</c:v>
+                  <c:v>35.145000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>39.05</c:v>
+                  <c:v>39.049999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6F0E-F24F-B5C6-EBDF34150446}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2722,19 +2743,19 @@
                   <c:v>3.5145</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.686</c:v>
+                  <c:v>4.6859999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.8575</c:v>
+                  <c:v>5.8574999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.029</c:v>
+                  <c:v>7.0289999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.2005</c:v>
+                  <c:v>8.2004999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.372</c:v>
+                  <c:v>9.3719999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>10.5435</c:v>
@@ -2746,6 +2767,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6F0E-F24F-B5C6-EBDF34150446}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2792,7 +2818,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2913,7 +2938,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2943,6 +2967,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2991,10 +3016,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.248850462962963"/>
-          <c:y val="0.915711342592593"/>
-          <c:w val="0.536151851851852"/>
-          <c:h val="0.0554893518518518"/>
+          <c:x val="0.24885046296296301"/>
+          <c:y val="0.91571134259259301"/>
+          <c:w val="0.53615185185185199"/>
+          <c:h val="5.5489351851851797E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3064,7 +3089,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3103,7 +3128,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3172,22 +3196,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90.0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110.0</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120.0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>130.0</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3202,15 +3226,20 @@
                   <c:v>7.35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28.975</c:v>
+                  <c:v>28.975000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F860-C847-9CE8-C7E9817596AE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3245,22 +3274,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90.0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110.0</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120.0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>130.0</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3272,18 +3301,23 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.205</c:v>
+                  <c:v>2.2050000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8575</c:v>
+                  <c:v>5.8574999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.6925</c:v>
+                  <c:v>8.6925000000000008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F860-C847-9CE8-C7E9817596AE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3330,7 +3364,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3408,7 +3441,7 @@
         <c:axId val="1106895280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="30.0"/>
+          <c:max val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3452,7 +3485,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3482,6 +3514,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3530,10 +3563,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.242468287037037"/>
+          <c:x val="0.24246828703703699"/>
           <c:y val="0.886794444444444"/>
-          <c:w val="0.57300527193137"/>
-          <c:h val="0.0894555360674702"/>
+          <c:w val="0.57300527193136996"/>
+          <c:h val="8.9455536067470198E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3603,7 +3636,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3642,7 +3675,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3711,27 +3743,32 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1880-5444-AC42-EA7016E84085}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3766,13 +3803,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.9525</c:v>
+                  <c:v>1.9524999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.905</c:v>
+                  <c:v>3.9049999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8575</c:v>
+                  <c:v>5.8574999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7.81</c:v>
@@ -3781,12 +3818,17 @@
                   <c:v>11.715</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1880-5444-AC42-EA7016E84085}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3833,7 +3875,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3954,7 +3995,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3984,6 +4024,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4032,10 +4073,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.248850462962963"/>
-          <c:y val="0.909831712962963"/>
-          <c:w val="0.536151851851852"/>
-          <c:h val="0.0554893518518518"/>
+          <c:x val="0.24885046296296301"/>
+          <c:y val="0.90983171296296295"/>
+          <c:w val="0.53615185185185199"/>
+          <c:h val="5.5489351851851797E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4105,7 +4146,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4144,7 +4185,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4212,7 +4252,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>18.45</c:v>
@@ -4220,6 +4260,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A317-294F-B08F-C38F8D9C09CD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4252,14 +4297,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5.8575</c:v>
+                  <c:v>5.8574999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.535</c:v>
+                  <c:v>5.5350000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A317-294F-B08F-C38F8D9C09CD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4306,7 +4356,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4427,7 +4476,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4457,6 +4505,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4505,10 +4554,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.422299537037037"/>
-          <c:y val="0.906891898148148"/>
+          <c:x val="0.42229953703703699"/>
+          <c:y val="0.90689189814814797"/>
           <c:w val="0.217339583333333"/>
-          <c:h val="0.0554893518518518"/>
+          <c:h val="5.5489351851851797E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4578,7 +4627,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4617,7 +4666,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4709,24 +4757,29 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.525</c:v>
+                  <c:v>19.524999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DE64-BB40-B25D-6B7D889CACF0}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4784,24 +4837,29 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.8575</c:v>
+                  <c:v>5.8574999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.8575</c:v>
+                  <c:v>5.8574999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8575</c:v>
+                  <c:v>5.8574999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8575</c:v>
+                  <c:v>5.8574999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.8575</c:v>
+                  <c:v>5.8574999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DE64-BB40-B25D-6B7D889CACF0}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4848,7 +4906,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4969,7 +5026,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4999,6 +5055,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5047,10 +5104,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.240031018518519"/>
-          <c:y val="0.901012268518518"/>
-          <c:w val="0.536151851851852"/>
-          <c:h val="0.0554893518518518"/>
+          <c:x val="0.24003101851851899"/>
+          <c:y val="0.90101226851851801"/>
+          <c:w val="0.53615185185185199"/>
+          <c:h val="5.5489351851851797E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -10140,7 +10197,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -10172,7 +10235,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -10204,7 +10273,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -10236,7 +10311,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -10273,7 +10354,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -10303,7 +10390,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -10335,7 +10428,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -10367,7 +10466,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -10399,7 +10504,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -10681,11 +10792,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J143"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="J143" sqref="J143"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10726,7 +10837,7 @@
     <row r="7" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>28</v>
       </c>
     </row>
@@ -10734,10 +10845,10 @@
       <c r="A10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>25</v>
       </c>
     </row>
@@ -10745,49 +10856,49 @@
       <c r="A11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="19">
         <v>80</v>
       </c>
-      <c r="C11" s="24">
-        <v>-32</v>
+      <c r="C11" s="23">
+        <v>-70</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
-      <c r="B12" s="20">
+      <c r="B12" s="19">
         <v>90</v>
       </c>
-      <c r="C12" s="24"/>
+      <c r="C12" s="23"/>
     </row>
     <row r="13" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
-      <c r="B13" s="20">
+      <c r="B13" s="19">
         <v>100</v>
       </c>
-      <c r="C13" s="24"/>
+      <c r="C13" s="23"/>
     </row>
     <row r="14" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="19">
         <v>110</v>
       </c>
-      <c r="C14" s="24">
-        <v>-11</v>
+      <c r="C14" s="23">
+        <v>-30</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="20">
+      <c r="B15" s="19">
         <v>120</v>
       </c>
-      <c r="C15" s="24"/>
+      <c r="C15" s="23"/>
     </row>
     <row r="16" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="21">
+      <c r="B16" s="20">
         <v>130</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="24">
         <v>-4</v>
       </c>
     </row>
@@ -10795,19 +10906,19 @@
       <c r="B17" s="1"/>
     </row>
     <row r="18" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="26">
         <f>C16-C11</f>
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="29"/>
+      <c r="C19" s="28"/>
     </row>
     <row r="20" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
@@ -10842,7 +10953,7 @@
     <row r="38" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="21" t="s">
         <v>28</v>
       </c>
     </row>
@@ -10850,10 +10961,10 @@
       <c r="A41" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="23" t="s">
+      <c r="C41" s="22" t="s">
         <v>26</v>
       </c>
     </row>
@@ -10861,49 +10972,49 @@
       <c r="A42" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="20">
+      <c r="B42" s="19">
         <v>80</v>
       </c>
-      <c r="C42" s="24">
+      <c r="C42" s="23">
         <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="14"/>
-      <c r="B43" s="20">
+      <c r="B43" s="19">
         <v>90</v>
       </c>
-      <c r="C43" s="24"/>
+      <c r="C43" s="23"/>
     </row>
     <row r="44" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="14"/>
-      <c r="B44" s="20">
+      <c r="B44" s="19">
         <v>100</v>
       </c>
-      <c r="C44" s="24"/>
+      <c r="C44" s="23"/>
     </row>
     <row r="45" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="20">
+      <c r="B45" s="19">
         <v>110</v>
       </c>
-      <c r="C45" s="24">
+      <c r="C45" s="23">
         <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="20">
+      <c r="B46" s="19">
         <v>120</v>
       </c>
-      <c r="C46" s="24"/>
+      <c r="C46" s="23"/>
     </row>
     <row r="47" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="21">
+      <c r="B47" s="20">
         <v>130</v>
       </c>
-      <c r="C47" s="25">
+      <c r="C47" s="24">
         <v>46</v>
       </c>
     </row>
@@ -10911,19 +11022,19 @@
       <c r="B48" s="1"/>
     </row>
     <row r="49" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="27">
+      <c r="C49" s="26">
         <f>C47-C42</f>
         <v>7</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="28" t="s">
+      <c r="B50" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C50" s="29"/>
+      <c r="C50" s="28"/>
     </row>
     <row r="51" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="1"/>
@@ -10955,7 +11066,7 @@
     <row r="68" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="69" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="70" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="22" t="s">
+      <c r="C70" s="21" t="s">
         <v>28</v>
       </c>
     </row>
@@ -10963,10 +11074,10 @@
       <c r="A71" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B71" s="19" t="s">
+      <c r="B71" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C71" s="23" t="s">
+      <c r="C71" s="22" t="s">
         <v>29</v>
       </c>
     </row>
@@ -10974,49 +11085,49 @@
       <c r="A72" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B72" s="20">
+      <c r="B72" s="19">
         <v>80</v>
       </c>
-      <c r="C72" s="24">
+      <c r="C72" s="23">
         <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="14"/>
-      <c r="B73" s="20">
+      <c r="B73" s="19">
         <v>90</v>
       </c>
-      <c r="C73" s="24"/>
+      <c r="C73" s="23"/>
     </row>
     <row r="74" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="14"/>
-      <c r="B74" s="20">
+      <c r="B74" s="19">
         <v>100</v>
       </c>
-      <c r="C74" s="24"/>
+      <c r="C74" s="23"/>
     </row>
     <row r="75" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B75" s="20">
+      <c r="B75" s="19">
         <v>110</v>
       </c>
-      <c r="C75" s="24">
+      <c r="C75" s="23">
         <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="20">
+      <c r="B76" s="19">
         <v>120</v>
       </c>
-      <c r="C76" s="24"/>
+      <c r="C76" s="23"/>
     </row>
     <row r="77" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="21">
+      <c r="B77" s="20">
         <v>130</v>
       </c>
-      <c r="C77" s="25">
+      <c r="C77" s="24">
         <v>73</v>
       </c>
     </row>
@@ -11034,19 +11145,19 @@
     </row>
     <row r="80" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="81" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="26" t="s">
+      <c r="B81" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C81" s="27">
+      <c r="C81" s="26">
         <f>C77-C72</f>
         <v>-4</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="28" t="s">
+      <c r="B82" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C82" s="29"/>
+      <c r="C82" s="28"/>
     </row>
     <row r="83" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="84" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11064,7 +11175,7 @@
     <row r="96" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="99" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="100" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C100" s="22" t="s">
+      <c r="C100" s="21" t="s">
         <v>28</v>
       </c>
     </row>
@@ -11072,10 +11183,10 @@
       <c r="A101" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B101" s="19" t="s">
+      <c r="B101" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C101" s="23" t="s">
+      <c r="C101" s="22" t="s">
         <v>27</v>
       </c>
     </row>
@@ -11083,49 +11194,49 @@
       <c r="A102" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B102" s="20">
+      <c r="B102" s="19">
         <v>80</v>
       </c>
-      <c r="C102" s="24">
+      <c r="C102" s="23">
         <v>1192</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="14"/>
-      <c r="B103" s="20">
+      <c r="B103" s="19">
         <v>90</v>
       </c>
-      <c r="C103" s="24"/>
+      <c r="C103" s="23"/>
     </row>
     <row r="104" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="14"/>
-      <c r="B104" s="20">
+      <c r="B104" s="19">
         <v>100</v>
       </c>
-      <c r="C104" s="24"/>
+      <c r="C104" s="23"/>
     </row>
     <row r="105" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B105" s="20">
+      <c r="B105" s="19">
         <v>110</v>
       </c>
-      <c r="C105" s="24">
+      <c r="C105" s="23">
         <v>909</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B106" s="20">
+      <c r="B106" s="19">
         <v>120</v>
       </c>
-      <c r="C106" s="24"/>
+      <c r="C106" s="23"/>
     </row>
     <row r="107" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="21">
+      <c r="B107" s="20">
         <v>130</v>
       </c>
-      <c r="C107" s="25">
+      <c r="C107" s="24">
         <v>787</v>
       </c>
     </row>
@@ -11143,19 +11254,19 @@
     </row>
     <row r="110" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="111" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B111" s="26" t="s">
+      <c r="B111" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C111" s="30">
+      <c r="C111" s="29">
         <f>C107-C102</f>
         <v>-405</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="31" t="s">
+      <c r="B112" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C112" s="32"/>
+      <c r="C112" s="31"/>
     </row>
     <row r="113" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="114" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11189,7 +11300,7 @@
       <c r="B137" t="s">
         <v>34</v>
       </c>
-      <c r="J137" s="33"/>
+      <c r="J137" s="32"/>
     </row>
     <row r="138" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A138" s="6"/>
@@ -11201,7 +11312,7 @@
       <c r="B139" t="s">
         <v>35</v>
       </c>
-      <c r="J139" s="33"/>
+      <c r="J139" s="32"/>
     </row>
     <row r="140" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="141" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -11211,7 +11322,7 @@
       <c r="B141" t="s">
         <v>47</v>
       </c>
-      <c r="J141" s="33"/>
+      <c r="J141" s="32"/>
     </row>
     <row r="142" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="143" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -11221,7 +11332,7 @@
       <c r="B143" t="s">
         <v>46</v>
       </c>
-      <c r="J143" s="33"/>
+      <c r="J143" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11231,7 +11342,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L175"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A152" workbookViewId="0">
@@ -11916,7 +12027,7 @@
         <v>38</v>
       </c>
       <c r="D162"/>
-      <c r="J162" s="33"/>
+      <c r="J162" s="32"/>
     </row>
     <row r="163" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A163" s="6"/>
@@ -11930,7 +12041,7 @@
         <v>39</v>
       </c>
       <c r="D164"/>
-      <c r="J164" s="33"/>
+      <c r="J164" s="32"/>
     </row>
     <row r="165" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A165" s="6"/>
@@ -11943,7 +12054,7 @@
         <v>40</v>
       </c>
       <c r="D166"/>
-      <c r="J166" s="33"/>
+      <c r="J166" s="32"/>
     </row>
     <row r="167" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A167" s="6"/>
@@ -11955,24 +12066,24 @@
       <c r="B168" t="s">
         <v>43</v>
       </c>
-      <c r="E168" s="38"/>
-      <c r="F168" s="39"/>
-      <c r="G168" s="39"/>
-      <c r="H168" s="39"/>
-      <c r="I168" s="39"/>
-      <c r="J168" s="39"/>
-      <c r="K168" s="39"/>
-      <c r="L168" s="40"/>
+      <c r="E168" s="37"/>
+      <c r="F168" s="38"/>
+      <c r="G168" s="38"/>
+      <c r="H168" s="38"/>
+      <c r="I168" s="38"/>
+      <c r="J168" s="38"/>
+      <c r="K168" s="38"/>
+      <c r="L168" s="39"/>
     </row>
     <row r="169" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A169" s="6"/>
-      <c r="E169" s="41"/>
-      <c r="F169" s="18"/>
-      <c r="G169" s="18"/>
-      <c r="H169" s="18"/>
-      <c r="I169" s="18"/>
-      <c r="J169" s="18"/>
-      <c r="K169" s="18"/>
+      <c r="E169" s="40"/>
+      <c r="F169" s="41"/>
+      <c r="G169" s="41"/>
+      <c r="H169" s="41"/>
+      <c r="I169" s="41"/>
+      <c r="J169" s="41"/>
+      <c r="K169" s="41"/>
       <c r="L169" s="42"/>
     </row>
     <row r="170" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -11985,27 +12096,27 @@
       <c r="B171" t="s">
         <v>44</v>
       </c>
-      <c r="E171" s="38"/>
-      <c r="F171" s="39"/>
-      <c r="G171" s="39"/>
-      <c r="H171" s="39"/>
-      <c r="I171" s="39"/>
-      <c r="J171" s="39"/>
-      <c r="K171" s="39"/>
-      <c r="L171" s="40"/>
+      <c r="E171" s="37"/>
+      <c r="F171" s="38"/>
+      <c r="G171" s="38"/>
+      <c r="H171" s="38"/>
+      <c r="I171" s="38"/>
+      <c r="J171" s="38"/>
+      <c r="K171" s="38"/>
+      <c r="L171" s="39"/>
     </row>
     <row r="172" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A172" s="6"/>
       <c r="B172" t="s">
         <v>45</v>
       </c>
-      <c r="E172" s="41"/>
-      <c r="F172" s="18"/>
-      <c r="G172" s="18"/>
-      <c r="H172" s="18"/>
-      <c r="I172" s="18"/>
-      <c r="J172" s="18"/>
-      <c r="K172" s="18"/>
+      <c r="E172" s="40"/>
+      <c r="F172" s="41"/>
+      <c r="G172" s="41"/>
+      <c r="H172" s="41"/>
+      <c r="I172" s="41"/>
+      <c r="J172" s="41"/>
+      <c r="K172" s="41"/>
       <c r="L172" s="42"/>
     </row>
     <row r="173" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -12018,27 +12129,27 @@
       <c r="B174" t="s">
         <v>41</v>
       </c>
-      <c r="E174" s="34"/>
-      <c r="F174" s="35"/>
-      <c r="G174" s="35"/>
-      <c r="H174" s="35"/>
-      <c r="I174" s="35"/>
-      <c r="J174" s="35"/>
-      <c r="K174" s="35"/>
-      <c r="L174" s="27"/>
+      <c r="E174" s="33"/>
+      <c r="F174" s="34"/>
+      <c r="G174" s="34"/>
+      <c r="H174" s="34"/>
+      <c r="I174" s="34"/>
+      <c r="J174" s="34"/>
+      <c r="K174" s="34"/>
+      <c r="L174" s="26"/>
     </row>
     <row r="175" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>42</v>
       </c>
-      <c r="E175" s="36"/>
-      <c r="F175" s="37"/>
-      <c r="G175" s="37"/>
-      <c r="H175" s="37"/>
-      <c r="I175" s="37"/>
-      <c r="J175" s="37"/>
-      <c r="K175" s="37"/>
-      <c r="L175" s="29"/>
+      <c r="E175" s="35"/>
+      <c r="F175" s="36"/>
+      <c r="G175" s="36"/>
+      <c r="H175" s="36"/>
+      <c r="I175" s="36"/>
+      <c r="J175" s="36"/>
+      <c r="K175" s="36"/>
+      <c r="L175" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -12052,7 +12163,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
fix for dose info
</commit_message>
<xml_diff>
--- a/CT_Sim_Workbook_V1.xlsx
+++ b/CT_Sim_Workbook_V1.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnstowe/CTSim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D9CE8E-F37C-064F-8C1B-1516283DB3E1}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A43431B7-D563-344C-943D-5FE837B1678F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25020" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24880" windowHeight="15540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dual Energy" sheetId="3" r:id="rId1"/>
     <sheet name="Doses" sheetId="1" r:id="rId2"/>
-    <sheet name="Noise" sheetId="2" r:id="rId3"/>
+    <sheet name="ToDo" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
   <si>
     <t>Graphing of Dose vs CT Parameters</t>
   </si>
@@ -174,6 +174,21 @@
   </si>
   <si>
     <t>Is there a significant difference in soft tissue values close to water ( i.e. 0 HU) as the kVp increases?</t>
+  </si>
+  <si>
+    <t>Task 6</t>
+  </si>
+  <si>
+    <t>Spatial Resolution</t>
+  </si>
+  <si>
+    <t>Contrast Resolution</t>
+  </si>
+  <si>
+    <t>Noise</t>
+  </si>
+  <si>
+    <t>Other explorations</t>
   </si>
 </sst>
 </file>
@@ -903,7 +918,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EEB8-CE41-9B81-21D1E6DC8520}"/>
+              <c16:uniqueId val="{00000000-FF18-EB44-B78D-A2884320F80F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1316,10 +1331,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-70</c:v>
+                  <c:v>-32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-30</c:v>
+                  <c:v>-11</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-4</c:v>
@@ -1330,7 +1345,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4F04-8A44-9060-3EE48C95595A}"/>
+              <c16:uniqueId val="{00000000-562B-EA45-B0A8-0421D3B3EE5F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1762,7 +1777,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-01EF-6448-ABFC-94B6F73EEAAF}"/>
+              <c16:uniqueId val="{00000000-4DEE-9F41-865D-49D23D34C1E0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2235,7 +2250,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-94A5-ED4E-9ECB-B93D3314BD8F}"/>
+              <c16:uniqueId val="{00000000-B9C4-5146-9AB2-5B2532F8F448}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2697,7 +2712,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6F0E-F24F-B5C6-EBDF34150446}"/>
+              <c16:uniqueId val="{00000000-C858-B343-A889-3BEE87E6D37A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2769,7 +2784,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6F0E-F24F-B5C6-EBDF34150446}"/>
+              <c16:uniqueId val="{00000001-C858-B343-A889-3BEE87E6D37A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3237,7 +3252,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F860-C847-9CE8-C7E9817596AE}"/>
+              <c16:uniqueId val="{00000000-1081-0E41-82F5-4942D29684D7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3315,7 +3330,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F860-C847-9CE8-C7E9817596AE}"/>
+              <c16:uniqueId val="{00000001-1081-0E41-82F5-4942D29684D7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3766,7 +3781,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1880-5444-AC42-EA7016E84085}"/>
+              <c16:uniqueId val="{00000000-3AE2-3645-93F9-0E473B711E1B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3826,7 +3841,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1880-5444-AC42-EA7016E84085}"/>
+              <c16:uniqueId val="{00000001-3AE2-3645-93F9-0E473B711E1B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4245,6 +4260,21 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Doses!$B$131:$B$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Doses!$C$131:$C$132</c:f>
@@ -4262,7 +4292,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A317-294F-B08F-C38F8D9C09CD}"/>
+              <c16:uniqueId val="{00000000-31F6-B344-9C1B-B2A1C94A50CB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4290,6 +4320,21 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Doses!$B$131:$B$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Doses!$D$131:$D$132</c:f>
@@ -4307,7 +4352,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A317-294F-B08F-C38F8D9C09CD}"/>
+              <c16:uniqueId val="{00000001-31F6-B344-9C1B-B2A1C94A50CB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4777,7 +4822,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DE64-BB40-B25D-6B7D889CACF0}"/>
+              <c16:uniqueId val="{00000000-45AC-754E-AF6C-D5D3425A1F86}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4857,7 +4902,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-DE64-BB40-B25D-6B7D889CACF0}"/>
+              <c16:uniqueId val="{00000001-45AC-754E-AF6C-D5D3425A1F86}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10795,8 +10840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J143"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="J143" sqref="J143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10860,7 +10905,7 @@
         <v>80</v>
       </c>
       <c r="C11" s="23">
-        <v>-70</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -10885,7 +10930,7 @@
         <v>110</v>
       </c>
       <c r="C14" s="23">
-        <v>-30</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -10911,7 +10956,7 @@
       </c>
       <c r="C18" s="26">
         <f>C16-C11</f>
-        <v>66</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -11345,8 +11390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L175"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="G160" sqref="G160"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="A160" sqref="A160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12008,7 +12053,7 @@
     <row r="159" spans="1:4" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="160" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="13" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B160" s="13" t="s">
         <v>33</v>
@@ -12164,12 +12209,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>